<commit_message>
minor changes to UI
</commit_message>
<xml_diff>
--- a/sampleSpreadsheet.xlsx
+++ b/sampleSpreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ericx\Documents\dev\david-steven-eric\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FFAA858-364A-41F3-8288-2C7BC1B6D0E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3A9BD53-0B39-4DFA-B4F6-52C7D5D26C1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{836594FC-68A9-460B-8AAE-FCA68522931D}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>3HGGK5H88KM742051</t>
   </si>
@@ -43,6 +43,9 @@
   </si>
   <si>
     <t>JTDKARFP5J3103946</t>
+  </si>
+  <si>
+    <t>1FMCU9GD1HUA30879</t>
   </si>
 </sst>
 </file>
@@ -395,10 +398,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C144B6EC-AC97-45AB-ADA1-F61A2B03E922}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -439,6 +442,17 @@
         <v>20000</v>
       </c>
     </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>18000</v>
+      </c>
+      <c r="C4" s="1">
+        <v>25000</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
US-16, refer to readme
</commit_message>
<xml_diff>
--- a/sampleSpreadsheet.xlsx
+++ b/sampleSpreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ericx\Documents\dev\david-steven-eric\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7A6A644-2BA3-48DB-BBE0-09B6B31F9DD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B76BC654-24BC-45E2-8ACE-8B16A0F7ECB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{836594FC-68A9-460B-8AAE-FCA68522931D}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="13">
   <si>
     <t>3HGGK5H88KM742051</t>
   </si>
@@ -64,6 +64,15 @@
   </si>
   <si>
     <t>1LN6L9NP1J5616818</t>
+  </si>
+  <si>
+    <t>For sale</t>
+  </si>
+  <si>
+    <t>In-transit</t>
+  </si>
+  <si>
+    <t>Sold</t>
   </si>
 </sst>
 </file>
@@ -416,10 +425,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C144B6EC-AC97-45AB-ADA1-F61A2B03E922}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:C10"/>
+      <selection activeCell="D8" sqref="D8:D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -427,7 +436,7 @@
     <col min="1" max="1" width="23.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -437,8 +446,11 @@
       <c r="C1" s="1">
         <v>19000</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -448,8 +460,11 @@
       <c r="C2" s="1">
         <v>20000</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -459,8 +474,11 @@
       <c r="C3" s="1">
         <v>20000</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -470,8 +488,11 @@
       <c r="C4" s="1">
         <v>19000</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -481,8 +502,11 @@
       <c r="C5" s="1">
         <v>20000</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -492,8 +516,11 @@
       <c r="C6" s="1">
         <v>20000</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -503,8 +530,11 @@
       <c r="C7" s="1">
         <v>19000</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -514,8 +544,11 @@
       <c r="C8" s="1">
         <v>20000</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -525,8 +558,11 @@
       <c r="C9" s="1">
         <v>20000</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -535,6 +571,9 @@
       </c>
       <c r="C10" s="1">
         <v>20000</v>
+      </c>
+      <c r="D10" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed issue with trailing spaces with spreadsheet upload by using trim function
</commit_message>
<xml_diff>
--- a/sampleSpreadsheet.xlsx
+++ b/sampleSpreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ericx\Documents\dev\david-steven-eric\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAE7061B-1577-44E2-9728-31E33F8FB660}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4753B2A2-18C2-49C0-A4B6-2263E494B1A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34365" yWindow="2145" windowWidth="21600" windowHeight="11235" xr2:uid="{836594FC-68A9-460B-8AAE-FCA68522931D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{836594FC-68A9-460B-8AAE-FCA68522931D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -90,19 +90,19 @@
     <t>SADCJ2BN5HA086947</t>
   </si>
   <si>
+    <t>5NPD84LF6KH490922</t>
+  </si>
+  <si>
+    <t>5npe34af3jh646547</t>
+  </si>
+  <si>
+    <t>55SWF4KB5GU142000</t>
+  </si>
+  <si>
+    <t>3HGGK5H82KM719817</t>
+  </si>
+  <si>
     <t xml:space="preserve">KNMAT2MV3JP608780 </t>
-  </si>
-  <si>
-    <t>5NPD84LF6KH490922</t>
-  </si>
-  <si>
-    <t>5npe34af3jh646547</t>
-  </si>
-  <si>
-    <t>55SWF4KB5GU142000</t>
-  </si>
-  <si>
-    <t>3HGGK5H82KM719817</t>
   </si>
 </sst>
 </file>
@@ -457,8 +457,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C144B6EC-AC97-45AB-ADA1-F61A2B03E922}">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A20"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -723,7 +723,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B16" s="1">
         <v>15000</v>
@@ -740,7 +740,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B17" s="1">
         <v>17000</v>
@@ -757,7 +757,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B18" s="1">
         <v>16000</v>
@@ -774,7 +774,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B19" s="1">
         <v>15000</v>
@@ -791,7 +791,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B20" s="1">
         <v>15000</v>

</xml_diff>